<commit_message>
Fixed random words selection, decreased block size.
</commit_message>
<xml_diff>
--- a/development/stimuli/word_lists/art_distractors_ORIGINAL.xlsx
+++ b/development/stimuli/word_lists/art_distractors_ORIGINAL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\codes\subliminal_priming\stimuli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\development\stimuli\word_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357D35A0-4229-4FD8-AB12-7B3D7B730F26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3E2DB6-702E-4675-95B1-B7ABD7621148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="31">
   <si>
     <t>עניבה</t>
   </si>
@@ -127,36 +127,6 @@
   </si>
   <si>
     <t>יאכטה</t>
-  </si>
-  <si>
-    <t>שקר1</t>
-  </si>
-  <si>
-    <t>שקר2</t>
-  </si>
-  <si>
-    <t>שקר3</t>
-  </si>
-  <si>
-    <t>שקר4</t>
-  </si>
-  <si>
-    <t>שקר5</t>
-  </si>
-  <si>
-    <t>שקר6</t>
-  </si>
-  <si>
-    <t>שקר7</t>
-  </si>
-  <si>
-    <t>שקר8</t>
-  </si>
-  <si>
-    <t>שקר9</t>
-  </si>
-  <si>
-    <t>שקר10</t>
   </si>
 </sst>
 </file>
@@ -651,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD46"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1989,39 +1959,17 @@
       <c r="L15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="N15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="O15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="P15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="R15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="S15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="T15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="U15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="V15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="W15" s="16" t="s">
-        <v>31</v>
-      </c>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
       <c r="X15" s="1" t="s">
         <v>24</v>
       </c>
@@ -2081,39 +2029,17 @@
       <c r="L16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="N16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="O16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="P16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="R16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="S16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="T16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="U16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="V16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="W16" s="16" t="s">
-        <v>32</v>
-      </c>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
       <c r="X16" s="1" t="s">
         <v>19</v>
       </c>
@@ -2173,39 +2099,17 @@
       <c r="L17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="N17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="O17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="P17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="R17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="S17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="T17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="U17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="V17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="W17" s="16" t="s">
-        <v>33</v>
-      </c>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
       <c r="X17" s="1" t="s">
         <v>8</v>
       </c>
@@ -2265,39 +2169,17 @@
       <c r="L18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="N18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="O18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="P18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="R18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="S18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="T18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="U18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="V18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="W18" s="16" t="s">
-        <v>34</v>
-      </c>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="16"/>
       <c r="X18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2357,39 +2239,17 @@
       <c r="L19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="N19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="O19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="P19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="R19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="S19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="T19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="U19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="V19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="W19" s="16" t="s">
-        <v>35</v>
-      </c>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="16"/>
       <c r="X19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2449,39 +2309,17 @@
       <c r="L20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="N20" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="O20" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="P20" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q20" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="R20" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="S20" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="T20" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="U20" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="V20" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="W20" s="16" t="s">
-        <v>36</v>
-      </c>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="16"/>
       <c r="X20" s="1" t="s">
         <v>19</v>
       </c>
@@ -2541,39 +2379,17 @@
       <c r="L21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="N21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="O21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="P21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="R21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="S21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="U21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="V21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="W21" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="16"/>
       <c r="X21" s="1" t="s">
         <v>26</v>
       </c>
@@ -2633,39 +2449,17 @@
       <c r="L22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="N22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="O22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="P22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="R22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="S22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="T22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="U22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="V22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="W22" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="16"/>
       <c r="X22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2725,39 +2519,17 @@
       <c r="L23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="N23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="O23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="P23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="R23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="S23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="T23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="U23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="V23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="W23" s="16" t="s">
-        <v>39</v>
-      </c>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
       <c r="X23" s="1" t="s">
         <v>1</v>
       </c>
@@ -2817,39 +2589,17 @@
       <c r="L24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M24" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="N24" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="O24" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="P24" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q24" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="R24" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="S24" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="T24" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="U24" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="V24" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="W24" s="16" t="s">
-        <v>40</v>
-      </c>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="16"/>
       <c r="X24" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>